<commit_message>
1.5.5: Updated Documentation/GCA_Improvement_List.xls with current progress. Updated Bug Reports/Memory Trace X-Axis Rescale Problem documents to reflect the fact that segmented sweeps are effected. Ready to give this version to Jerome for evaluation.
</commit_message>
<xml_diff>
--- a/Documentation/GCA_Improvement_List.xlsx
+++ b/Documentation/GCA_Improvement_List.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lalic\Documents\Qt\PACompressionTest\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lalic\Documents\Qt\PACompressionTest\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="888" yWindow="0" windowWidth="28800" windowHeight="14232"/>
+    <workbookView xWindow="1815" yWindow="0" windowWidth="28800" windowHeight="14235"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
   <si>
     <t>Category</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Move plots to a different figure</t>
   </si>
   <si>
-    <t>Resolve the scaling issue caused by a change in measurement conditions</t>
-  </si>
-  <si>
     <t>End of sweep conditions (RF Off with power displayed at the bottom of plots)</t>
   </si>
   <si>
@@ -122,12 +119,6 @@
     <t>In Progress</t>
   </si>
   <si>
-    <t>I was able to reproduce and document this phenomenon. Unfortunately, it is an issue with our VNA firmware. I generated a report to send to our firmware developers. I will update you when I get a response, and I will continue to think of a work-around in the meantime.</t>
-  </si>
-  <si>
-    <t>This depends on a development team in Munich. I can make the request, but I don't know if/when it would get implemented. A work-around Greg recommended is to display the power range in the diagram title. Not sure if that would work. Another idea is to use markers to display the ranges.</t>
-  </si>
-  <si>
     <t>Not started</t>
   </si>
   <si>
@@ -137,19 +128,37 @@
     <t>In progress</t>
   </si>
   <si>
-    <t>vs Pin, Pout plot points are x10</t>
-  </si>
-  <si>
     <t>1.5.5</t>
   </si>
   <si>
-    <t>Finished testing the various trace combinations, but I couldn't reproduce the intermittent error when plotting vs Pout. I did fix an issue you saw when moving from one X-axis type to another (say Pin to Frequency, and vice versa). Unfortunately the fix for now is for me to delete then recreate the trace entirely. I expect this will only need to be done when configuring the setup initially, so it shouldn't be a huge issue.</t>
-  </si>
-  <si>
     <t>On hold for critical bug fixes.</t>
   </si>
   <si>
-    <t>A message is generated, and the value is rounded to the nearest valid value.</t>
+    <t>FWIW, also added phase of Pin (0 deg)</t>
+  </si>
+  <si>
+    <t>1.5.5*</t>
+  </si>
+  <si>
+    <t>1.5.6</t>
+  </si>
+  <si>
+    <t>I was able to reproduce and document this phenomenon. Unfortunately, it is an issue with our VNA firmware. I generated a report to send to our firmware developers. I will update you when I get a response. A work-around would be for me to delete then recreate the trace entirely, but this would mean that you'd have to re-setup the plots (not convenient).</t>
+  </si>
+  <si>
+    <t>Finished testing the various trace combinations, but I couldn't reproduce the intermittent error when plotting vs Pout. I did fix an issue you saw when moving from one X-axis type to another (say Pin to Frequency, and vice versa). Unfortunately the fix for now is for me to delete then recreate the trace entirely. I expect these trace changes will only need to be done during the initial configuration, so hopefully this isn't a big issue.</t>
+  </si>
+  <si>
+    <t>vs Pin, Pout plots have 10x points</t>
+  </si>
+  <si>
+    <t>This depends on the development team in Munich. I can make the request, but I don't know if/when it would get implemented. A work-around Greg recommended is to display the power range in the diagram title. Not sure if that would work since in general the ranges in the diagram may not all be the same. Another idea is to use markers at the trace endpoints.</t>
+  </si>
+  <si>
+    <t>Resolve the x-axis scaling issue caused by a change in measurement conditions</t>
+  </si>
+  <si>
+    <t>The GUI will not let you input incorrect values: any at value that is not possible is rounded to the nearest possible value. If you watch the value as you enter it, you should see this. That said, I will add a warning in the next version.</t>
   </si>
 </sst>
 </file>
@@ -602,20 +611,20 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="71.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="71.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="40.44140625" customWidth="1"/>
-    <col min="6" max="6" width="67.33203125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="40.42578125" customWidth="1"/>
+    <col min="6" max="6" width="67.28515625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -629,33 +638,33 @@
         <v>12</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -666,32 +675,34 @@
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="F3" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="E4" s="6"/>
       <c r="F4" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -702,14 +713,16 @@
         <v>3</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="F5" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -720,48 +733,54 @@
         <v>3</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="F6" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="E7" s="6"/>
       <c r="F7" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4"/>
+      <c r="D8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="F8" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -772,12 +791,14 @@
         <v>2</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -788,12 +809,14 @@
         <v>2</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -804,12 +827,14 @@
         <v>2</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -820,12 +845,14 @@
         <v>2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -836,28 +863,32 @@
         <v>2</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="11"/>
-    </row>
-    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="E14" s="6"/>
       <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -868,14 +899,14 @@
         <v>2</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="E15" s="6"/>
       <c r="F15" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -886,32 +917,32 @@
         <v>2</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="E16" s="6"/>
       <c r="F16" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="E17" s="6"/>
       <c r="F17" s="11"/>
     </row>
-    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="5"/>
     </row>

</xml_diff>